<commit_message>
nouvelle ligne dans le fichier d'import xlsx
</commit_message>
<xml_diff>
--- a/fichier_type_import_utilisateurs.xlsx
+++ b/fichier_type_import_utilisateurs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NoguesS\OneDrive - Facylities Multi Services\Documents\Emma40\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TibatiG\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC43C97-DB24-4CFA-A1A3-F8E0F93EAB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FADCE9-072A-4658-A7FE-E9D51D8D2C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29484" yWindow="4512" windowWidth="21600" windowHeight="11292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Matricule</t>
   </si>
@@ -75,13 +75,40 @@
   </si>
   <si>
     <t>Type d'accès</t>
+  </si>
+  <si>
+    <t>De Banville</t>
+  </si>
+  <si>
+    <t>Théodore</t>
+  </si>
+  <si>
+    <t>theo2b@poete.fr</t>
+  </si>
+  <si>
+    <t>Jean Paul Sartre</t>
+  </si>
+  <si>
+    <t>jps@jpsmedia.fr</t>
+  </si>
+  <si>
+    <t>Poète</t>
+  </si>
+  <si>
+    <t>Expression Lyrique</t>
+  </si>
+  <si>
+    <t>Albi</t>
+  </si>
+  <si>
+    <t>Restreint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -92,6 +119,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,14 +144,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,8 +473,8 @@
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -479,8 +515,47 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10102008</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <v>81000</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{68DA9BC0-7C6C-4552-B7B4-518E3A3BB12E}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{342B9B62-9FAA-4921-B275-3C95470792EC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>